<commit_message>
Added making folders, lists, entries and cleaned up data
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -45,8 +45,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -390,10 +396,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C6"/>
+      <selection activeCell="A9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -445,63 +451,114 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Wypisuje zawartośc listy</t>
+          <t>Wypisuje zawartość listy</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>nazwa listy, domyślnie czynnosci</t>
+          <t>nazwa listy, domyślnie main</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>newpointcounter</t>
+          <t>addlist</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dodaje użytkownika do bazy danych z punktami</t>
+          <t>Dodaje liste</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>nazwa użytkownika, domyślnie użytkownik wysyłający polecenie</t>
+          <t>nazwa listy</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>addpoint</t>
+          <t>addentries</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Dodaje użytkownikowi punkt</t>
+          <t>Dodaje wpisy do listy</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>nazwa użytkownika, domyślnie użytkownik wysyłający polecenie</t>
+          <t>nazwa listy, ilosc powtórzeń wpisu, wpis</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>newpointcounter</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Dodaje użytkownika do bazy danych z punktami</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>nazwa użytkownika, domyślnie użytkownik wysyłający polecenie</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>addpoint</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Dodaje użytkownikowi punkt</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>nazwa użytkownika, domyślnie użytkownik wysyłający polecenie</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>getpoints</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Pokazuje ilośc punktów dla użytkownika</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Pokazuje ilość punktów dla użytkownika</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>nazwa użytkownika, domyślnie użytkownik wysyłający polecenie</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="36" customHeight="1">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>makebase</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>Dodaje folder użytkownikowi, jeśli folder ten wcześniej nie istniał</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>brak</t>
         </is>
       </c>
     </row>

</xml_diff>